<commit_message>
Other examples to test the code added
</commit_message>
<xml_diff>
--- a/MATLAB_code/EXAMPLE_YUAN.xlsx
+++ b/MATLAB_code/EXAMPLE_YUAN.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datos\Desktop\Jaswant\Tesis\Matlab\codigo de yuang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Prestress_finding\MATLAB_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAD928E-DD8B-49A2-9D1D-EC5DC18D29DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5142E8-4537-4326-932A-E7B5CB9611FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF281D0E-6D1A-43DA-82B4-AFEE9B19A75F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="CONNECTIVITY" sheetId="1" r:id="rId1"/>
+    <sheet name="COORDINATES" sheetId="2" r:id="rId2"/>
+    <sheet name="FREE NODES" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>